<commit_message>
Thêm chức năng chia data
</commit_message>
<xml_diff>
--- a/public/files/template/Mau_nhap_data_mkt.xlsx
+++ b/public/files/template/Mau_nhap_data_mkt.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338861A3-31B8-47F0-A12D-B84C38A19595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -262,7 +263,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -363,9 +364,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -403,9 +404,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -440,7 +441,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -475,7 +476,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -648,11 +649,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,11 +955,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1042,10 +1043,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" display="http://crm.forewin.vn/xadmin-document/product-group/form/id/15729465663748uj816060/"/>
-    <hyperlink ref="G4" r:id="rId2" display="http://crm.forewin.vn/xadmin-document/product-group/form/id/1572946558a139uob6652z/"/>
-    <hyperlink ref="G5" r:id="rId3" display="http://crm.forewin.vn/xadmin-document/product-group/form/id/1572946531861t403m5307/"/>
-    <hyperlink ref="G6" r:id="rId4" display="http://crm.forewin.vn/xadmin-document/product-group/form/id/1573114979a0wj63k9y97m/"/>
+    <hyperlink ref="G3" r:id="rId1" display="http://crm.forewin.vn/xadmin-document/product-group/form/id/15729465663748uj816060/" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G4" r:id="rId2" display="http://crm.forewin.vn/xadmin-document/product-group/form/id/1572946558a139uob6652z/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="G5" r:id="rId3" display="http://crm.forewin.vn/xadmin-document/product-group/form/id/1572946531861t403m5307/" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="G6" r:id="rId4" display="http://crm.forewin.vn/xadmin-document/product-group/form/id/1573114979a0wj63k9y97m/" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>

</xml_diff>

<commit_message>
Thêm sản phẩm quan tâm khi import data mkt
</commit_message>
<xml_diff>
--- a/public/files/template/Mau_nhap_data_mkt.xlsx
+++ b/public/files/template/Mau_nhap_data_mkt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338861A3-31B8-47F0-A12D-B84C38A19595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB08D97-4D48-4C05-BA5A-BB3BFA6679D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="20685" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
   <si>
     <t>STT</t>
   </si>
@@ -96,22 +96,10 @@
     <t>Sản phẩm quan tâm</t>
   </si>
   <si>
-    <t>Thảm ô tô</t>
-  </si>
-  <si>
-    <t>Phủ nano</t>
-  </si>
-  <si>
     <t>Có thể điền bất kỳ ký tự nào</t>
   </si>
   <si>
     <t>Giới hạn là 10 số</t>
-  </si>
-  <si>
-    <t>Taplo ô tô</t>
-  </si>
-  <si>
-    <t>Thiết bị theo dõi</t>
   </si>
   <si>
     <t>(Có thể có thêm các Nhóm sản phẩm mới khi bổ sung trong cấu hình trên)</t>
@@ -258,6 +246,12 @@
   </si>
   <si>
     <t>Định dạng ngày dd/mm/yyyy hh:mm:ss</t>
+  </si>
+  <si>
+    <t>Thảm 5D 6D</t>
+  </si>
+  <si>
+    <t>Thảm TPE</t>
   </si>
 </sst>
 </file>
@@ -652,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,16 +681,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -704,7 +698,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -719,13 +713,13 @@
         <v>22</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -733,7 +727,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>8</v>
@@ -748,13 +742,13 @@
         <v>23</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -762,7 +756,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
@@ -777,13 +771,13 @@
         <v>24</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -791,7 +785,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
@@ -806,13 +800,13 @@
         <v>23</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -820,7 +814,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>11</v>
@@ -835,117 +829,117 @@
         <v>23</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="G7" s="4" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="G8" s="4" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="H8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="G9" s="4" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>30</v>
+      <c r="G10" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -957,10 +951,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,57 +992,41 @@
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G3" s="6" t="s">
-        <v>27</v>
+      <c r="G3" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G4" s="6" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G5" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G6" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G7" t="s">
-        <v>32</v>
+      <c r="G5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" display="http://crm.forewin.vn/xadmin-document/product-group/form/id/15729465663748uj816060/" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="G4" r:id="rId2" display="http://crm.forewin.vn/xadmin-document/product-group/form/id/1572946558a139uob6652z/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="G5" r:id="rId3" display="http://crm.forewin.vn/xadmin-document/product-group/form/id/1572946531861t403m5307/" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="G6" r:id="rId4" display="http://crm.forewin.vn/xadmin-document/product-group/form/id/1573114979a0wj63k9y97m/" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sửa file mẫu import data mkt
</commit_message>
<xml_diff>
--- a/public/files/template/Mau_nhap_data_mkt.xlsx
+++ b/public/files/template/Mau_nhap_data_mkt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB08D97-4D48-4C05-BA5A-BB3BFA6679D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639829E9-3605-42EC-9282-7C0A43A874E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="20685" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="20685" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
   <si>
     <t>STT</t>
   </si>
@@ -140,9 +140,6 @@
     <t>0355230187</t>
   </si>
   <si>
-    <t>0355230188</t>
-  </si>
-  <si>
     <t>Nguyễn Huy Hoàng 1</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>Nguyễn Huy Hoàng 3</t>
   </si>
   <si>
-    <t>Nguyễn Huy Hoàng 4</t>
-  </si>
-  <si>
     <t>MayBach 63</t>
   </si>
   <si>
@@ -164,9 +158,6 @@
     <t>MayBach 65</t>
   </si>
   <si>
-    <t>MayBach 66</t>
-  </si>
-  <si>
     <t>Bọc full Cốp</t>
   </si>
   <si>
@@ -176,9 +167,6 @@
     <t>Bọc thảm</t>
   </si>
   <si>
-    <t>Mua thêm nguyên vật liệu</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nội dung </t>
   </si>
   <si>
@@ -209,9 +197,6 @@
     <t>146 Cầu Giấy Hà Nội</t>
   </si>
   <si>
-    <t>147 Cầu Giấy Hà Nội</t>
-  </si>
-  <si>
     <t>Nghề nghiệp</t>
   </si>
   <si>
@@ -219,9 +204,6 @@
   </si>
   <si>
     <t>01/09/2019 08:15:50</t>
-  </si>
-  <si>
-    <t>4/11/2019 08:20:50</t>
   </si>
   <si>
     <t>3/11/2019 08:12:50</t>
@@ -646,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,16 +663,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -698,7 +680,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -713,13 +695,13 @@
         <v>22</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -727,7 +709,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>8</v>
@@ -742,13 +724,13 @@
         <v>23</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -756,7 +738,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
@@ -771,13 +753,13 @@
         <v>24</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -785,7 +767,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
@@ -800,13 +782,13 @@
         <v>23</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -814,7 +796,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>11</v>
@@ -829,118 +811,95 @@
         <v>23</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="G10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -953,7 +912,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -992,7 +951,7 @@
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
@@ -1012,12 +971,12 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G3" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G4" s="6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
thêm cột sản phẩm quan tâm và liên hệ sale
</commit_message>
<xml_diff>
--- a/public/files/template/Mau_nhap_data_mkt.xlsx
+++ b/public/files/template/Mau_nhap_data_mkt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639829E9-3605-42EC-9282-7C0A43A874E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9A2520-1162-45EE-BC6D-D0AD3DA9565F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="20685" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="3765" windowWidth="20685" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -629,7 +629,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>